<commit_message>
v2.3 10806 har score
</commit_message>
<xml_diff>
--- a/v2.3_SFN_Covariates.xlsx
+++ b/v2.3_SFN_Covariates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avidachs/Documents/GitHub/rf1-sra-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528B7AA8-72B2-1E47-AA4B-18E0DD21A790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48E4C13-5E5B-444E-A3D6-8E4E36C89302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{E21B9450-44FE-AB4C-A453-866E41E6C653}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{E21B9450-44FE-AB4C-A453-866E41E6C653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5055" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5054" uniqueCount="201">
   <si>
     <t>tania_subid</t>
   </si>
@@ -998,10 +998,10 @@
   <dimension ref="A1:GB90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BZ5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CB46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CJ21" sqref="CJ21"/>
+      <selection pane="bottomRight" activeCell="CI69" sqref="CI69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38389,8 +38389,8 @@
       <c r="CH68">
         <v>50</v>
       </c>
-      <c r="CI68" t="s">
-        <v>133</v>
+      <c r="CI68">
+        <v>22</v>
       </c>
       <c r="CJ68">
         <v>31</v>

</xml_diff>

<commit_message>
v2.3 10806 har and 10668 hvlt 0 to NaN
</commit_message>
<xml_diff>
--- a/v2.3_SFN_Covariates.xlsx
+++ b/v2.3_SFN_Covariates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avidachs/Documents/GitHub/rf1-sra-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48E4C13-5E5B-444E-A3D6-8E4E36C89302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF9F6A3-6498-2142-80D0-84C854E81077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{E21B9450-44FE-AB4C-A453-866E41E6C653}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5054" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5055" uniqueCount="201">
   <si>
     <t>tania_subid</t>
   </si>
@@ -998,10 +998,10 @@
   <dimension ref="A1:GB90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CB46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CI69" sqref="CI69"/>
+      <selection pane="bottomRight" activeCell="CE25" sqref="CE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22314,8 +22314,8 @@
       <c r="CE39" t="s">
         <v>133</v>
       </c>
-      <c r="CF39">
-        <v>0</v>
+      <c r="CF39" t="s">
+        <v>133</v>
       </c>
       <c r="CG39" t="s">
         <v>133</v>

</xml_diff>